<commit_message>
commit on Day 6
</commit_message>
<xml_diff>
--- a/ANSARI_ZAID_DAY_05_17TH_OCTOBER_2016.xlsx
+++ b/ANSARI_ZAID_DAY_05_17TH_OCTOBER_2016.xlsx
@@ -91,10 +91,10 @@
     <t>session bean factory deprecated</t>
   </si>
   <si>
-    <t>session bean factory is showing depre3cated</t>
-  </si>
-  <si>
     <t>session bean factory in hibernate 5 is available but auto import mechanism imports hibernate 3 version that give deprecation error so we have to change import to version  5</t>
+  </si>
+  <si>
+    <t>session bean factory is showing deprecated</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,10 +769,10 @@
     <row r="3" spans="1:4" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="D3" s="10"/>
     </row>

</xml_diff>